<commit_message>
Cut over improved min_model_M to tests/multialgorithm/fixtures/; switched on DEBUG-level debug logging.
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_model_for_exponential_growth_in_M.xlsx
+++ b/tests/multialgorithm/fixtures/test_model_for_exponential_growth_in_M.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aes/dev/gitroot/Karr_Lab/h1_hesc/cell_cycle/tyson_2011/hybrid_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4387FF17-38DF-A847-991C-0171E6029D32}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BF8A396-CDAD-0A4A-BA36-E1ADEE3EA26F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="2240" windowWidth="27000" windowHeight="7880" tabRatio="695" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -327,7 +327,7 @@
     <t>ln(2)/23 h</t>
   </si>
   <si>
-    <t>growthRate * M[c]</t>
+    <t>(growthRate/3600) * M[c]</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1667,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Fixed test_dynamic_components.py :: TestInitialRate_dM test case; incorporated 1/3600 h/s factor into test_model_for_exponential_growth_in_M.xlsx model parameter.
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_model_for_exponential_growth_in_M.xlsx
+++ b/tests/multialgorithm/fixtures/test_model_for_exponential_growth_in_M.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aes/dev/gitroot/Karr_Lab/h1_hesc/cell_cycle/tyson_2011/hybrid_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BF8A396-CDAD-0A4A-BA36-E1ADEE3EA26F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D3CBA658-210F-914D-8D1D-3B34684D9B9C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="2240" windowWidth="27000" windowHeight="7880" tabRatio="695" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="2240" windowWidth="27000" windowHeight="7880" tabRatio="695" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -324,10 +324,10 @@
     <t>growthRate</t>
   </si>
   <si>
-    <t>ln(2)/23 h</t>
-  </si>
-  <si>
-    <t>(growthRate/3600) * M[c]</t>
+    <t>growthRate * M[c]</t>
+  </si>
+  <si>
+    <t>ln(2)/23 h * 1 h / 3600 s = ln(2)/(23*3600) 1/s = 8.3713e-06 1/s</t>
   </si>
 </sst>
 </file>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -853,7 +853,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -970,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1049,14 +1049,14 @@
       <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="E3">
-        <v>3.0099999999999998E-2</v>
+      <c r="E3" s="6">
+        <v>8.3713000000000006E-6</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed test_dynamic_components.py :: TestInitialRate_dM test case; incorporated 1/3600 h/s factor into test_model_for_exponential_growth_in_M.xlsx model growthRate parameter.
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_model_for_exponential_growth_in_M.xlsx
+++ b/tests/multialgorithm/fixtures/test_model_for_exponential_growth_in_M.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aes/dev/gitroot/Karr_Lab/h1_hesc/cell_cycle/tyson_2011/hybrid_model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BF8A396-CDAD-0A4A-BA36-E1ADEE3EA26F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D3CBA658-210F-914D-8D1D-3B34684D9B9C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="2240" windowWidth="27000" windowHeight="7880" tabRatio="695" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1360" yWindow="2240" windowWidth="27000" windowHeight="7880" tabRatio="695" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -324,10 +324,10 @@
     <t>growthRate</t>
   </si>
   <si>
-    <t>ln(2)/23 h</t>
-  </si>
-  <si>
-    <t>(growthRate/3600) * M[c]</t>
+    <t>growthRate * M[c]</t>
+  </si>
+  <si>
+    <t>ln(2)/23 h * 1 h / 3600 s = ln(2)/(23*3600) 1/s = 8.3713e-06 1/s</t>
   </si>
 </sst>
 </file>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -853,7 +853,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -970,7 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1049,14 +1049,14 @@
       <c r="D3" t="s">
         <v>82</v>
       </c>
-      <c r="E3">
-        <v>3.0099999999999998E-2</v>
+      <c r="E3" s="6">
+        <v>8.3713000000000006E-6</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>